<commit_message>
Fixing some minor changes
</commit_message>
<xml_diff>
--- a/src/main/resources/conversion_table.xlsx
+++ b/src/main/resources/conversion_table.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="UACVDB01_SQL2008EXPRESS_StopNet4_3_tblConversionMark_56" localSheetId="0" hidden="1">Лист1!$A$1:$F$58</definedName>
+    <definedName name="UACVDB01_SQL2008EXPRESS_StopNet4_3_tblConversionMark_56" localSheetId="0" hidden="1">Лист1!$A$1:$F$54</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="191">
   <si>
     <t>colMarkID</t>
   </si>
@@ -63,9 +63,6 @@
     <t>н</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>рв</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
     <t>День без оплати</t>
   </si>
   <si>
-    <t>Прогул</t>
-  </si>
-  <si>
     <t>БЛ</t>
   </si>
   <si>
@@ -342,9 +336,6 @@
     <t>Відпустка по догляду до 6-ти років</t>
   </si>
   <si>
-    <t>Вихідний</t>
-  </si>
-  <si>
     <t>ТО</t>
   </si>
   <si>
@@ -603,7 +594,16 @@
     <t>вихідні</t>
   </si>
   <si>
-    <t>вихідний</t>
+    <t>Выгружать (yes|no)</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Часов по умолчанию(0 - значить вычислять из табеля)</t>
   </si>
 </sst>
 </file>
@@ -709,8 +709,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="UACVDB01_SQL2008EXPRESS StopNet4_3 tblConversionMark_56" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="10" unboundColumnsRight="3">
-    <queryTableFields count="9">
+  <queryTableRefresh nextId="12" unboundColumnsRight="5">
+    <queryTableFields count="11">
       <queryTableField id="1" name="colMarkID" tableColumnId="1"/>
       <queryTableField id="2" name="colMark" tableColumnId="2"/>
       <queryTableField id="3" name="colDescription" tableColumnId="3"/>
@@ -720,15 +720,17 @@
       <queryTableField id="8" dataBound="0" tableColumnId="7"/>
       <queryTableField id="7" dataBound="0" tableColumnId="8"/>
       <queryTableField id="9" dataBound="0" tableColumnId="9"/>
+      <queryTableField id="10" dataBound="0" tableColumnId="10"/>
+      <queryTableField id="11" dataBound="0" tableColumnId="11"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_UACVDB01_SQL2008EXPRESS_StopNet4_3_tblConversionMark_56" displayName="Table_UACVDB01_SQL2008EXPRESS_StopNet4_3_tblConversionMark_56" ref="A1:I58" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:I58"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_UACVDB01_SQL2008EXPRESS_StopNet4_3_tblConversionMark_56" displayName="Table_UACVDB01_SQL2008EXPRESS_StopNet4_3_tblConversionMark_56" ref="A1:K54" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:K54"/>
+  <tableColumns count="11">
     <tableColumn id="1" uniqueName="1" name="colMarkID" queryTableFieldId="1"/>
     <tableColumn id="2" uniqueName="2" name="StopNet" queryTableFieldId="2"/>
     <tableColumn id="3" uniqueName="3" name="colDescription" queryTableFieldId="3"/>
@@ -740,6 +742,8 @@
     <tableColumn id="9" uniqueName="9" name="Column3" queryTableFieldId="9" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(G:G,Sheet1!A:C,3,0)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="10" uniqueName="10" name="Выгружать (yes|no)" queryTableFieldId="10"/>
+    <tableColumn id="11" uniqueName="11" name="Часов по умолчанию(0 - значить вычислять из табеля)" queryTableFieldId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1008,29 +1012,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="156.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.140625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="83.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1045,16 +1051,22 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" t="s">
         <v>187</v>
       </c>
-      <c r="H1" t="s">
-        <v>185</v>
-      </c>
-      <c r="I1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1084,8 +1096,14 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Години роботи, передбачені колдоговором</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1115,16 +1133,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Нічні години роботи</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1136,7 +1160,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
@@ -1146,16 +1170,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Години роботи у вихідні й святкові дні</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>188</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1167,88 +1197,106 @@
         <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I5" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи, передбачені колдоговором</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Відрядження</v>
+      </c>
+      <c r="J5" t="s">
+        <v>188</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
+      <c r="H6" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>27</v>
+      </c>
+      <c r="I6" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Неоплачувана тимчасова непрацездатність у випадках, передбачених законодавством (побутова травма й т.п.)</v>
+      </c>
+      <c r="J6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
         <v>100</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>7</v>
-      </c>
-      <c r="I6" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Відрядження</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
       </c>
       <c r="F7">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="H7" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I7" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Неоплачувана тимчасова непрацездатність у випадках, передбачених законодавством (побутова травма й т.п.)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Неявки по нез'ясованих причинах</v>
+      </c>
+      <c r="J7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1257,29 +1305,35 @@
         <v>100</v>
       </c>
       <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
         <v>8</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H8" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>28</v>
-      </c>
       <c r="I8" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Неявки по нез'ясованих причинах</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Відпустка основна щорічна (ст. 6 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J8" t="s">
+        <v>188</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1291,23 +1345,29 @@
         <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H9" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>14</v>
+      </c>
+      <c r="I9" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Додаткова відпустка без збереження заробітної плати (ст. 25 крім п. 3, 12, 13, 17 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J9" t="s">
+        <v>188</v>
+      </c>
+      <c r="K9">
         <v>8</v>
       </c>
-      <c r="I9" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Відпустка основна щорічна (ст. 6 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -1322,69 +1382,81 @@
         <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="H10" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>12</v>
+      </c>
+      <c r="I10" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Додаткова відпустка у зв'язку з навчанням (ст. 13, 14, 15 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J10" t="s">
+        <v>188</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>14</v>
       </c>
-      <c r="I10" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Додаткова відпустка без збереження заробітної плати (ст. 25 крім п. 3, 12, 13, 17 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>13</v>
-      </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F11">
         <v>4</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>9</v>
+        <v>143</v>
       </c>
       <c r="H11" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Додаткова відпустка у зв'язку з навчанням (ст. 13, 14, 15 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Відпустка без збереження заробітної плати у зв'язку з навчанням (п. 12, 13, 17 ст. 25  Закону України "Про відпустки")</v>
+      </c>
+      <c r="J11" t="s">
+        <v>188</v>
+      </c>
+      <c r="K11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>4</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H12" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
@@ -1394,16 +1466,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Відпустка без збереження заробітної плати у зв'язку з навчанням (п. 12, 13, 17 ст. 25  Закону України "Про відпустки")</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>188</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1415,26 +1493,32 @@
         <v>4</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>146</v>
+        <v>10</v>
       </c>
       <c r="H13" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I13" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Відпустка без збереження заробітної плати у зв'язку з навчанням (п. 12, 13, 17 ст. 25  Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Години роботи у вихідні й святкові дні</v>
+      </c>
+      <c r="J13" t="s">
+        <v>189</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1446,57 +1530,69 @@
         <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="H14" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="I14" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи у вихідні й святкові дні</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Відпустка у зв'язку з вагітністю й пологами (ст. 17 Закону України "Про відпустки") і відпустка по догляду за дитиною до 3 років (ст. 18 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J14" t="s">
+        <v>188</v>
+      </c>
+      <c r="K14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F15">
         <v>4</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="H15" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I15" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Відпустка у зв'язку з вагітністю й пологами (ст. 17 Закону України "Про відпустки") і відпустка по догляду за дитиною до 3 років (ст. 18 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Інший невідпрацьований час, передбачений законодавством</v>
+      </c>
+      <c r="J15" t="s">
+        <v>189</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1508,7 +1604,7 @@
         <v>4</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H16" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
@@ -1518,16 +1614,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Інший невідпрацьований час, передбачений законодавством</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>189</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1539,7 +1641,7 @@
         <v>4</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H17" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
@@ -1549,19 +1651,25 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Інший невідпрацьований час, передбачений законодавством</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>189</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>100</v>
@@ -1570,63 +1678,75 @@
         <v>4</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>139</v>
+        <v>37</v>
       </c>
       <c r="H18" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I18" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Інший невідпрацьований час, передбачений законодавством</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Години роботи працівникам, яким установлений неповний робочий день (тиждень) згідно законодавства</v>
+      </c>
+      <c r="J18" t="s">
+        <v>189</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="H19" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="I19" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи працівникам, яким установлений неповний робочий день (тиждень) згідно законодавства</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Додаткова відпустка без збереження заробітної плати (ст. 25 крім п. 3, 12, 13, 17 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J19" t="s">
+        <v>188</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>4</v>
@@ -1642,16 +1762,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Години роботи, передбачені колдоговором</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>189</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1663,26 +1789,32 @@
         <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H21" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="I21" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Додаткова відпустка без збереження заробітної плати (ст. 25 крім п. 3, 12, 13, 17 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Неоплачувана тимчасова непрацездатність у випадках, передбачених законодавством (побутова травма й т.п.)</v>
+      </c>
+      <c r="J21" t="s">
+        <v>189</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1694,26 +1826,32 @@
         <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="H22" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="I22" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи, передбачені колдоговором</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Інші відпустки без збереження заробітної плати</v>
+      </c>
+      <c r="J22" t="s">
+        <v>188</v>
+      </c>
+      <c r="K22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1725,29 +1863,35 @@
         <v>4</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="H23" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I23" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Неоплачувана тимчасова непрацездатність у випадках, передбачених законодавством (побутова травма й т.п.)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Інші відпустки без збереження заробітної плати</v>
+      </c>
+      <c r="J23" t="s">
+        <v>188</v>
+      </c>
+      <c r="K23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1756,26 +1900,32 @@
         <v>4</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="H24" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I24" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Інші відпустки без збереження заробітної плати</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Простої</v>
+      </c>
+      <c r="J24" t="s">
+        <v>189</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1787,29 +1937,35 @@
         <v>4</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="H25" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="I25" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Інші відпустки без збереження заробітної плати</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Години роботи, передбачені колдоговором</v>
+      </c>
+      <c r="J25" t="s">
+        <v>189</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1818,26 +1974,32 @@
         <v>4</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>163</v>
+        <v>53</v>
       </c>
       <c r="H26" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I26" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Простої</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Прогули</v>
+      </c>
+      <c r="J26" t="s">
+        <v>189</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1859,16 +2021,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Години роботи, передбачені колдоговором</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>189</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1880,26 +2048,32 @@
         <v>4</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="H28" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="I28" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Прогули</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Години роботи, передбачені колдоговором</v>
+      </c>
+      <c r="J28" t="s">
+        <v>189</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1910,27 +2084,27 @@
       <c r="F29">
         <v>4</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>1</v>
-      </c>
-      <c r="I29" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи, передбачені колдоговором</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="1"/>
+      <c r="H29" s="2"/>
+      <c r="I29" t="s">
+        <v>186</v>
+      </c>
+      <c r="J29" t="s">
+        <v>189</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1942,51 +2116,69 @@
         <v>4</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
       <c r="H30" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I30" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи, передбачені колдоговором</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Масові невиходи на роботу (страйки)</v>
+      </c>
+      <c r="J30" t="s">
+        <v>189</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F31">
-        <v>4</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="2"/>
-      <c r="I31" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="I31" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Вечірні години роботи</v>
+      </c>
+      <c r="J31" t="s">
+        <v>188</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1998,26 +2190,32 @@
         <v>4</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="H32" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I32" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Масові невиходи на роботу (страйки)</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Інші види неявок</v>
+      </c>
+      <c r="J32" t="s">
+        <v>188</v>
+      </c>
+      <c r="K32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2029,57 +2227,69 @@
         <v>1</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="H33" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I33" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Вечірні години роботи</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Години роботи, передбачені колдоговором</v>
+      </c>
+      <c r="J33" t="s">
+        <v>189</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="H34" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="I34" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Інші види неявок</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Години роботи, передбачені колдоговором</v>
+      </c>
+      <c r="J34" t="s">
+        <v>189</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2101,16 +2311,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Години роботи, передбачені колдоговором</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>189</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2132,16 +2348,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Години роботи, передбачені колдоговором</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>189</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -2163,16 +2385,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Години роботи, передбачені колдоговором</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>189</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2194,16 +2422,22 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Години роботи, передбачені колдоговором</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>189</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -2212,35 +2446,41 @@
         <v>100</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="H39" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="I39" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи, передбачені колдоговором</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Простої</v>
+      </c>
+      <c r="J39" t="s">
+        <v>188</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -2256,140 +2496,170 @@
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Години роботи, передбачені колдоговором</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>189</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>100</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="H41" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I41" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Простої</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Оплачувана тимчасова непрацездатність</v>
+      </c>
+      <c r="J41" t="s">
+        <v>188</v>
+      </c>
+      <c r="K41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="H42" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I42" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи, передбачені колдоговором</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Відпустка у зв'язку з вагітністю й пологами (ст. 17 Закону України "Про відпустки") і відпустка по догляду за дитиною до 3 років (ст. 18 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J42" t="s">
+        <v>188</v>
+      </c>
+      <c r="K42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="H43" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I43" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Прогули</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Відпустка основна щорічна (ст. 6 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J43" t="s">
+        <v>188</v>
+      </c>
+      <c r="K43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C44" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>181</v>
+        <v>111</v>
       </c>
       <c r="H44" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I44" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Оплачувана тимчасова непрацездатність</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>Інші відпустки без збереження заробітної плати</v>
+      </c>
+      <c r="J44" t="s">
+        <v>188</v>
+      </c>
+      <c r="K44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2401,417 +2671,359 @@
         <v>1</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="H45" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>12</v>
+      </c>
+      <c r="I45" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Додаткова відпустка у зв'язку з навчанням (ст. 13, 14, 15 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J45" t="s">
+        <v>188</v>
+      </c>
+      <c r="K45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H46" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>15</v>
+      </c>
+      <c r="I46" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Додаткова оплачувана відпустка працівникам, що мають дітей (ст. 19 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J46" t="s">
+        <v>188</v>
+      </c>
+      <c r="K46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H47" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>19</v>
+      </c>
+      <c r="I47" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Інші відпустки без збереження заробітної плати</v>
+      </c>
+      <c r="J47" t="s">
+        <v>188</v>
+      </c>
+      <c r="K47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>104</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H48" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
         <v>16</v>
       </c>
-      <c r="I45" t="str">
+      <c r="I48" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Відпустка у зв'язку з вагітністю й пологами (ст. 17 Закону України "Про відпустки") і відпустка по догляду за дитиною до 3 років (ст. 18 Закону України "Про відпустки")</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>98</v>
-      </c>
-      <c r="B46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" t="s">
-        <v>90</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46">
+      <c r="J48" t="s">
+        <v>188</v>
+      </c>
+      <c r="K48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>105</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" t="s">
         <v>100</v>
       </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H46" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H49" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>17</v>
+      </c>
+      <c r="I49" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Відпустка по догляду за дитиною до 6 років (ст. 25 п. 3 Закону України "Про відпустки")</v>
+      </c>
+      <c r="J49" t="s">
+        <v>188</v>
+      </c>
+      <c r="K49">
         <v>8</v>
       </c>
-      <c r="I46" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Відпустка основна щорічна (ст. 6 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>108</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" t="s">
+        <v>102</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I50" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Години роботи, передбачені колдоговором</v>
+      </c>
+      <c r="J50" t="s">
+        <v>189</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>109</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
         <v>100</v>
       </c>
-      <c r="B47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H47" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>19</v>
-      </c>
-      <c r="I47" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Інші відпустки без збереження заробітної плати</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>101</v>
-      </c>
-      <c r="B48" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I51" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Години роботи, передбачені колдоговором</v>
+      </c>
+      <c r="J51" t="s">
+        <v>188</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>110</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
         <v>100</v>
       </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I52" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Години роботи, передбачені колдоговором</v>
+      </c>
+      <c r="J52" t="s">
+        <v>189</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>116</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53">
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>100</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H53" s="2">
+        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
+        <v>22</v>
+      </c>
+      <c r="I53" t="str">
+        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
+        <v>Інший невідпрацьований час, передбачений законодавством</v>
+      </c>
+      <c r="J53" t="s">
+        <v>188</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>119</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>100</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I48" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Додаткова відпустка у зв'язку з навчанням (ст. 13, 14, 15 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>102</v>
-      </c>
-      <c r="B49" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H49" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>15</v>
-      </c>
-      <c r="I49" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Додаткова оплачувана відпустка працівникам, що мають дітей (ст. 19 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>103</v>
-      </c>
-      <c r="B50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H50" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>19</v>
-      </c>
-      <c r="I50" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Інші відпустки без збереження заробітної плати</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>104</v>
-      </c>
-      <c r="B51" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H51" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>16</v>
-      </c>
-      <c r="I51" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Відпустка у зв'язку з вагітністю й пологами (ст. 17 Закону України "Про відпустки") і відпустка по догляду за дитиною до 3 років (ст. 18 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>105</v>
-      </c>
-      <c r="B52" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" t="s">
-        <v>102</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>1</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H52" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>17</v>
-      </c>
-      <c r="I52" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Відпустка по догляду за дитиною до 6 років (ст. 25 п. 3 Закону України "Про відпустки")</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>107</v>
-      </c>
-      <c r="B53" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" t="s">
-        <v>103</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="2"/>
-      <c r="I53" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>108</v>
-      </c>
-      <c r="B54" t="s">
-        <v>104</v>
-      </c>
-      <c r="C54" t="s">
-        <v>105</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="H54" s="2">
         <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I54" t="str">
         <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи, передбачені колдоговором</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>109</v>
-      </c>
-      <c r="B55" t="s">
-        <v>106</v>
-      </c>
-      <c r="C55" t="s">
-        <v>107</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>100</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H55" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>1</v>
-      </c>
-      <c r="I55" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи, передбачені колдоговором</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>110</v>
-      </c>
-      <c r="B56" t="s">
-        <v>108</v>
-      </c>
-      <c r="C56" t="s">
-        <v>109</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>100</v>
-      </c>
-      <c r="F56">
-        <v>1</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H56" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>1</v>
-      </c>
-      <c r="I56" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Години роботи, передбачені колдоговором</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>116</v>
-      </c>
-      <c r="B57" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57">
-        <v>4</v>
-      </c>
-      <c r="E57">
-        <v>100</v>
-      </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H57" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>22</v>
-      </c>
-      <c r="I57" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
-        <v>Інший невідпрацьований час, передбачений законодавством</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>119</v>
-      </c>
-      <c r="B58" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58" t="s">
-        <v>113</v>
-      </c>
-      <c r="D58">
-        <v>4</v>
-      </c>
-      <c r="E58">
-        <v>100</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" s="2">
-        <f>VLOOKUP(G:G,Sheet1!A:B,2,0)</f>
-        <v>7</v>
-      </c>
-      <c r="I58" t="str">
-        <f>VLOOKUP(G:G,Sheet1!A:C,3,0)</f>
         <v>Відрядження</v>
       </c>
+      <c r="J54" t="s">
+        <v>188</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H58">
-    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
+  <conditionalFormatting sqref="H2:H54">
+    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2825,7 +3037,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$30</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G58</xm:sqref>
+          <xm:sqref>G2:G54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2848,170 +3060,170 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B1">
         <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B9">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B10">
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B11">
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B12">
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3022,136 +3234,136 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B16">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B17">
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B19">
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D19" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B20">
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D20" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B21">
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D21" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22">
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3162,24 +3374,24 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D24" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3190,80 +3402,80 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D27" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B28">
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B29">
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D30" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>